<commit_message>
Changed the styling of a few things. Also, the functionality for the saving of the manual  mentee assignation has been improved. The button will change when changes are saved, but will a also change back when there are unsaved changes. On modal close, if changes are saved, all rows are unselected.
</commit_message>
<xml_diff>
--- a/src/frontend/data/mentors.xlsx
+++ b/src/frontend/data/mentors.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisarojas/GDrive/Graduate/Winter2018/CSCI5020G_Collaborative_Design_and_Research/project/repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisarojas/GDrive/Graduate/Winter2018/CSCI5020G_Collaborative_Design_and_Research/project/repo/src/frontend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B0C0F4-5C00-BA4D-9C04-23EC6270A06F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ECE5F5-D422-FA4B-A29F-56EFCE689ADC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="14560" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mentors (Made by Luisa)" sheetId="14" r:id="rId1"/>
+    <sheet name="Mentors" sheetId="14" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -1824,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90549B2-1AA3-BE46-90D8-E7C8AB09A7F5}">
   <dimension ref="A1:AF943"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12651,6 +12651,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046EA511BBCB59E42A88A619BFC75661B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="280e44903c962187b208735be74fa2e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -12782,25 +12800,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82426145-99DE-4CDC-81C2-FD828B0AADF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1782932A-B736-4F6B-91B2-C27EF01688B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0B7BE3-D1EB-49DA-AABC-5B30932E3CDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12816,28 +12840,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1782932A-B736-4F6B-91B2-C27EF01688B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82426145-99DE-4CDC-81C2-FD828B0AADF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>